<commit_message>
attacks and defenses tested on cluster
</commit_message>
<xml_diff>
--- a/result/celeb20.xlsx
+++ b/result/celeb20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anti-DreamBooth-Linux\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SD_benchmark\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C6FFFF-A9EC-4DE9-9281-FD6A8E701DA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F4BBF7-E112-4D58-8004-9153C202A5A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{0FFD3D56-ABFF-4DE3-B757-C5CDE37290D1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{0FFD3D56-ABFF-4DE3-B757-C5CDE37290D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3886,7 +3886,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I10"/>
+      <selection activeCell="A15" sqref="A15:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4344,39 +4344,39 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <f>B2-B10</f>
+        <f t="shared" ref="B16:I16" si="1">B2-B10</f>
         <v>-7.0400000000000018E-2</v>
       </c>
       <c r="C16">
-        <f>C2-C10</f>
+        <f t="shared" si="1"/>
         <v>9.6799999999999997E-2</v>
       </c>
       <c r="D16">
-        <f>D2-D10</f>
+        <f t="shared" si="1"/>
         <v>-0.1467</v>
       </c>
       <c r="E16">
-        <f>E2-E10</f>
+        <f t="shared" si="1"/>
         <v>-7.8099999999999947E-2</v>
       </c>
       <c r="F16">
-        <f>F2-F10</f>
+        <f t="shared" si="1"/>
         <v>-0.18869999999999998</v>
       </c>
       <c r="G16">
-        <f>G2-G10</f>
+        <f t="shared" si="1"/>
         <v>-7.8099999999999947E-2</v>
       </c>
       <c r="H16">
-        <f>H2-H10</f>
+        <f t="shared" si="1"/>
         <v>0.1991</v>
       </c>
       <c r="I16">
-        <f>I2-I10</f>
+        <f t="shared" si="1"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:J23" si="1">AVERAGE(B16:I16)</f>
+        <f t="shared" ref="J16:J23" si="2">AVERAGE(B16:I16)</f>
         <v>-8.2624999999999921E-3</v>
       </c>
     </row>
@@ -4385,39 +4385,39 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <f>B3-B10</f>
+        <f t="shared" ref="B17:I17" si="3">B3-B10</f>
         <v>-1.1299999999999977E-2</v>
       </c>
       <c r="C17">
-        <f>C3-C10</f>
+        <f t="shared" si="3"/>
         <v>0.15310000000000001</v>
       </c>
       <c r="D17">
-        <f>D3-D10</f>
+        <f t="shared" si="3"/>
         <v>-7.1099999999999941E-2</v>
       </c>
       <c r="E17">
-        <f>E3-E10</f>
+        <f t="shared" si="3"/>
         <v>-3.1200000000000006E-2</v>
       </c>
       <c r="F17">
-        <f>F3-F10</f>
+        <f t="shared" si="3"/>
         <v>-3.2100000000000017E-2</v>
       </c>
       <c r="G17">
-        <f>G3-G10</f>
+        <f t="shared" si="3"/>
         <v>0.10310000000000008</v>
       </c>
       <c r="H17">
-        <f>H3-H10</f>
+        <f t="shared" si="3"/>
         <v>0.2525</v>
       </c>
       <c r="I17">
-        <f>I3-I10</f>
+        <f t="shared" si="3"/>
         <v>0.27189999999999992</v>
       </c>
       <c r="J17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9362500000000002E-2</v>
       </c>
     </row>
@@ -4426,39 +4426,39 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <f>B4-B10</f>
+        <f t="shared" ref="B18:I18" si="4">B4-B10</f>
         <v>2.4599999999999955E-2</v>
       </c>
       <c r="C18">
-        <f>C4-C10</f>
+        <f t="shared" si="4"/>
         <v>-3.1999999999999806E-3</v>
       </c>
       <c r="D18">
-        <f>D4-D10</f>
+        <f t="shared" si="4"/>
         <v>2.5600000000000067E-2</v>
       </c>
       <c r="E18">
-        <f>E4-E10</f>
+        <f t="shared" si="4"/>
         <v>-3.1200000000000006E-2</v>
       </c>
       <c r="F18">
-        <f>F4-F10</f>
+        <f t="shared" si="4"/>
         <v>5.9000000000000163E-3</v>
       </c>
       <c r="G18">
-        <f>G4-G10</f>
+        <f t="shared" si="4"/>
         <v>-2.189999999999992E-2</v>
       </c>
       <c r="H18">
-        <f>H4-H10</f>
+        <f t="shared" si="4"/>
         <v>0.27999999999999997</v>
       </c>
       <c r="I18">
-        <f>I4-I10</f>
+        <f t="shared" si="4"/>
         <v>0.30309999999999993</v>
       </c>
       <c r="J18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2862499999999997E-2</v>
       </c>
     </row>
@@ -4467,39 +4467,39 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <f>B5-B10</f>
+        <f t="shared" ref="B19:I19" si="5">B5-B10</f>
         <v>0.15559999999999996</v>
       </c>
       <c r="C19">
-        <f>C5-C10</f>
+        <f t="shared" si="5"/>
         <v>0.23739999999999994</v>
       </c>
       <c r="D19">
-        <f>D5-D10</f>
+        <f t="shared" si="5"/>
         <v>4.2900000000000049E-2</v>
       </c>
       <c r="E19">
-        <f>E5-E10</f>
+        <f t="shared" si="5"/>
         <v>-2.5000000000000022E-2</v>
       </c>
       <c r="F19">
-        <f>F5-F10</f>
+        <f t="shared" si="5"/>
         <v>6.6899999999999959E-2</v>
       </c>
       <c r="G19">
-        <f>G5-G10</f>
+        <f t="shared" si="5"/>
         <v>0.28120000000000001</v>
       </c>
       <c r="H19">
-        <f>H5-H10</f>
+        <f t="shared" si="5"/>
         <v>0.3967</v>
       </c>
       <c r="I19">
-        <f>I5-I10</f>
+        <f t="shared" si="5"/>
         <v>0.32189999999999996</v>
       </c>
       <c r="J19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18469999999999998</v>
       </c>
     </row>
@@ -4508,39 +4508,39 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <f>B6-B10</f>
+        <f t="shared" ref="B20:I20" si="6">B6-B10</f>
         <v>-0.37960000000000005</v>
       </c>
       <c r="C20">
-        <f>C6-C10</f>
+        <f t="shared" si="6"/>
         <v>0.15620000000000001</v>
       </c>
       <c r="D20">
-        <f>D6-D10</f>
+        <f t="shared" si="6"/>
         <v>-0.49159999999999998</v>
       </c>
       <c r="E20">
-        <f>E6-E10</f>
+        <f t="shared" si="6"/>
         <v>-6.25E-2</v>
       </c>
       <c r="F20">
-        <f>F6-F10</f>
+        <f t="shared" si="6"/>
         <v>-0.37929999999999997</v>
       </c>
       <c r="G20">
-        <f>G6-G10</f>
+        <f t="shared" si="6"/>
         <v>0.23130000000000006</v>
       </c>
       <c r="H20">
-        <f>H6-H10</f>
+        <f t="shared" si="6"/>
         <v>-8.0600000000000005E-2</v>
       </c>
       <c r="I20">
-        <f>I6-I10</f>
+        <f t="shared" si="6"/>
         <v>0.22499999999999998</v>
       </c>
       <c r="J20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.7637500000000002E-2</v>
       </c>
     </row>
@@ -4549,39 +4549,39 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <f>B7-B10</f>
+        <f t="shared" ref="B21:I21" si="7">B7-B10</f>
         <v>0.13619999999999999</v>
       </c>
       <c r="C21">
-        <f>C7-C10</f>
+        <f t="shared" si="7"/>
         <v>0.27179999999999993</v>
       </c>
       <c r="D21">
-        <f>D7-D10</f>
+        <f t="shared" si="7"/>
         <v>6.2100000000000044E-2</v>
       </c>
       <c r="E21">
-        <f>E7-E10</f>
+        <f t="shared" si="7"/>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="F21">
-        <f>F7-F10</f>
+        <f t="shared" si="7"/>
         <v>5.3900000000000059E-2</v>
       </c>
       <c r="G21">
-        <f>G7-G10</f>
+        <f t="shared" si="7"/>
         <v>0.29380000000000006</v>
       </c>
       <c r="H21">
-        <f>H7-H10</f>
+        <f t="shared" si="7"/>
         <v>0.31460000000000005</v>
       </c>
       <c r="I21">
-        <f>I7-I10</f>
+        <f t="shared" si="7"/>
         <v>0.27499999999999991</v>
       </c>
       <c r="J21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17905000000000001</v>
       </c>
     </row>
@@ -4590,39 +4590,39 @@
         <v>5</v>
       </c>
       <c r="B22">
-        <f>B8-B10</f>
+        <f t="shared" ref="B22:I22" si="8">B8-B10</f>
         <v>0.14189999999999992</v>
       </c>
       <c r="C22">
-        <f>C8-C10</f>
+        <f t="shared" si="8"/>
         <v>0.21250000000000002</v>
       </c>
       <c r="D22">
-        <f>D8-D10</f>
+        <f t="shared" si="8"/>
         <v>4.7499999999999987E-2</v>
       </c>
       <c r="E22">
-        <f>E8-E10</f>
+        <f t="shared" si="8"/>
         <v>-4.3699999999999961E-2</v>
       </c>
       <c r="F22">
-        <f>F8-F10</f>
+        <f t="shared" si="8"/>
         <v>5.6100000000000039E-2</v>
       </c>
       <c r="G22">
-        <f>G8-G10</f>
+        <f t="shared" si="8"/>
         <v>0.16560000000000008</v>
       </c>
       <c r="H22">
-        <f>H8-H10</f>
+        <f t="shared" si="8"/>
         <v>0.34700000000000003</v>
       </c>
       <c r="I22">
-        <f>I8-I10</f>
+        <f t="shared" si="8"/>
         <v>0.30630000000000002</v>
       </c>
       <c r="J22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15415000000000001</v>
       </c>
     </row>
@@ -4631,39 +4631,39 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <f>B9-B10</f>
+        <f t="shared" ref="B23:I23" si="9">B9-B10</f>
         <v>4.0899999999999936E-2</v>
       </c>
       <c r="C23">
-        <f>C9-C10</f>
+        <f t="shared" si="9"/>
         <v>0.19989999999999997</v>
       </c>
       <c r="D23">
-        <f>D9-D10</f>
+        <f t="shared" si="9"/>
         <v>-5.0799999999999956E-2</v>
       </c>
       <c r="E23">
-        <f>E9-E10</f>
+        <f t="shared" si="9"/>
         <v>-5.9400000000000008E-2</v>
       </c>
       <c r="F23">
-        <f>F9-F10</f>
+        <f t="shared" si="9"/>
         <v>2.300000000000002E-2</v>
       </c>
       <c r="G23">
-        <f>G9-G10</f>
+        <f t="shared" si="9"/>
         <v>0.2219000000000001</v>
       </c>
       <c r="H23">
-        <f>H9-H10</f>
+        <f t="shared" si="9"/>
         <v>0.34920000000000001</v>
       </c>
       <c r="I23">
-        <f>I9-I10</f>
+        <f t="shared" si="9"/>
         <v>0.25629999999999997</v>
       </c>
       <c r="J23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12262500000000001</v>
       </c>
     </row>

</xml_diff>